<commit_message>
twik some parameters in gen algo for better solution
</commit_message>
<xml_diff>
--- a/schedule_genetic.xlsx
+++ b/schedule_genetic.xlsx
@@ -525,27 +525,27 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Автобус 2 (10:00 - 18:00)</t>
+          <t>Автобус 2 (06:00 - 14:00)</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>Автобус 2 (09:00 - 17:00)</t>
+          <t>Автобус 6 (07:00 - 15:00)</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>Автобус 5 (07:00 - 15:00)</t>
+          <t>Автобус 5 (09:00 - 17:00)</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>Автобус 5 (06:00 - 14:00)</t>
+          <t>Автобус 2 (07:00 - 15:00)</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
-          <t>Автобус 1 (09:00 - 17:00)</t>
+          <t>Автобус 8 (08:00 - 16:00)</t>
         </is>
       </c>
       <c r="H2" s="4" t="inlineStr">
@@ -572,27 +572,27 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Автобус 3 (10:00 - 18:00)</t>
+          <t>Автобус 1 (09:00 - 17:00)</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>Автобус 3 (06:00 - 14:00)</t>
+          <t>Автобус 7 (08:00 - 16:00)</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>Автобус 6 (09:00 - 17:00)</t>
+          <t>Автобус 2 (10:00 - 18:00)</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>Автобус 7 (09:00 - 17:00)</t>
+          <t>Автобус 8 (08:00 - 16:00)</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
         <is>
-          <t>Автобус 7 (06:00 - 14:00)</t>
+          <t>Автобус 7 (08:00 - 16:00)</t>
         </is>
       </c>
       <c r="H3" s="4" t="inlineStr">
@@ -619,27 +619,27 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Автобус 3 (10:00 - 18:00)</t>
+          <t>Автобус 6 (08:00 - 16:00)</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>Автобус 1 (10:00 - 18:00)</t>
+          <t>Автобус 4 (09:00 - 17:00)</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>Автобус 2 (06:00 - 14:00)</t>
+          <t>Автобус 6 (07:00 - 15:00)</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
+          <t>Автобус 3 (08:00 - 16:00)</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
           <t>Автобус 4 (10:00 - 18:00)</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
-        <is>
-          <t>Автобус 1 (06:00 - 14:00)</t>
         </is>
       </c>
       <c r="H4" s="4" t="inlineStr">
@@ -666,27 +666,27 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Автобус 6 (06:00 - 14:00)</t>
+          <t>Автобус 8 (09:00 - 17:00)</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>Автобус 2 (09:00 - 17:00)</t>
+          <t>Автобус 8 (06:00 - 14:00)</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>Автобус 8 (09:00 - 17:00)</t>
+          <t>Автобус 1 (09:00 - 17:00)</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>Автобус 7 (10:00 - 18:00)</t>
+          <t>Автобус 7 (09:00 - 17:00)</t>
         </is>
       </c>
       <c r="G5" s="3" t="inlineStr">
         <is>
-          <t>Автобус 6 (06:00 - 14:00)</t>
+          <t>Автобус 5 (06:00 - 14:00)</t>
         </is>
       </c>
       <c r="H5" s="4" t="inlineStr">
@@ -713,27 +713,27 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
+          <t>Автобус 5 (10:00 - 18:00)</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>Автобус 7 (07:00 - 15:00)</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>Автобус 4 (08:00 - 16:00)</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
           <t>Автобус 1 (10:00 - 18:00)</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>Автобус 2 (06:00 - 14:00)</t>
-        </is>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>Автобус 8 (06:00 - 14:00)</t>
-        </is>
-      </c>
-      <c r="F6" s="3" t="inlineStr">
-        <is>
-          <t>Автобус 2 (06:00 - 14:00)</t>
-        </is>
-      </c>
       <c r="G6" s="3" t="inlineStr">
         <is>
-          <t>Автобус 7 (10:00 - 18:00)</t>
+          <t>Автобус 2 (08:00 - 16:00)</t>
         </is>
       </c>
       <c r="H6" s="4" t="inlineStr">
@@ -760,27 +760,27 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
+          <t>Автобус 2 (08:00 - 16:00)</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>Автобус 4 (10:00 - 18:00)</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>Автобус 4 (06:00 - 14:00)</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>Автобус 8 (09:00 - 17:00)</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
           <t>Автобус 8 (08:00 - 16:00)</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>Автобус 4 (06:00 - 14:00)</t>
-        </is>
-      </c>
-      <c r="E7" s="3" t="inlineStr">
-        <is>
-          <t>Автобус 7 (07:00 - 15:00)</t>
-        </is>
-      </c>
-      <c r="F7" s="3" t="inlineStr">
-        <is>
-          <t>Автобус 4 (07:00 - 15:00)</t>
-        </is>
-      </c>
-      <c r="G7" s="3" t="inlineStr">
-        <is>
-          <t>Автобус 1 (09:00 - 17:00)</t>
         </is>
       </c>
       <c r="H7" s="4" t="inlineStr">
@@ -807,7 +807,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Автобус 5 (07:00 - 19:00)</t>
+          <t>Автобус 5 (10:00 - 22:00)</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -822,7 +822,7 @@
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>Автобус 8 (00:00 - 12:00)</t>
+          <t>Автобус 2 (09:00 - 21:00)</t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="I8" s="3" t="inlineStr">
         <is>
-          <t>Автобус 7 (04:00 - 16:00)</t>
+          <t>Автобус 1 (16:00 - 04:00)</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>Автобус 4 (10:00 - 22:00)</t>
+          <t>Автобус 8 (09:00 - 21:00)</t>
         </is>
       </c>
       <c r="D9" s="4" t="inlineStr">
@@ -884,7 +884,7 @@
       </c>
       <c r="I9" s="3" t="inlineStr">
         <is>
-          <t>Автобус 1 (04:00 - 16:00)</t>
+          <t>Автобус 1 (05:00 - 17:00)</t>
         </is>
       </c>
     </row>
@@ -906,7 +906,7 @@
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>Автобус 1 (19:00 - 07:00)</t>
+          <t>Автобус 5 (06:00 - 18:00)</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="G10" s="3" t="inlineStr">
         <is>
-          <t>Автобус 6 (23:00 - 11:00)</t>
+          <t>Автобус 7 (04:00 - 16:00)</t>
         </is>
       </c>
       <c r="H10" s="4" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>Автобус 1 (05:00 - 17:00)</t>
+          <t>Автобус 6 (10:00 - 22:00)</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>Автобус 5 (18:00 - 06:00)</t>
+          <t>Автобус 2 (07:00 - 19:00)</t>
         </is>
       </c>
       <c r="H11" s="4" t="inlineStr">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>Автобус 3 (13:00 - 01:00)</t>
+          <t>Автобус 8 (16:00 - 04:00)</t>
         </is>
       </c>
       <c r="F12" s="4" t="inlineStr">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="H12" s="3" t="inlineStr">
         <is>
-          <t>Автобус 7 (05:00 - 17:00)</t>
+          <t>Автобус 7 (15:00 - 03:00)</t>
         </is>
       </c>
       <c r="I12" s="4" t="inlineStr">
@@ -1052,7 +1052,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>Автобус 2 (08:00 - 20:00)</t>
+          <t>Автобус 6 (01:00 - 13:00)</t>
         </is>
       </c>
       <c r="F13" s="4" t="inlineStr">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>Автобус 4 (11:00 - 23:00)</t>
+          <t>Автобус 4 (05:00 - 17:00)</t>
         </is>
       </c>
       <c r="I13" s="4" t="inlineStr">

</xml_diff>